<commit_message>
Função para calcular a média da colocação dos últimos anos de cada equipe feita e início da implementação de grafos.
</commit_message>
<xml_diff>
--- a/position/flamengo.xlsx
+++ b/position/flamengo.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,6 +444,11 @@
           <t>Colocação</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Divisão</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -457,6 +462,11 @@
       <c r="C2" t="n">
         <v>5</v>
       </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Primeira Divisão</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -470,6 +480,11 @@
       <c r="C3" t="n">
         <v>2</v>
       </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Primeira Divisão</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -483,6 +498,11 @@
       <c r="C4" t="n">
         <v>1</v>
       </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Primeira Divisão</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -496,6 +516,11 @@
       <c r="C5" t="n">
         <v>1</v>
       </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Primeira Divisão</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -509,6 +534,11 @@
       <c r="C6" t="n">
         <v>2</v>
       </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Primeira Divisão</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -522,6 +552,11 @@
       <c r="C7" t="n">
         <v>6</v>
       </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Primeira Divisão</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -535,6 +570,11 @@
       <c r="C8" t="n">
         <v>3</v>
       </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Primeira Divisão</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -548,6 +588,11 @@
       <c r="C9" t="n">
         <v>12</v>
       </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Primeira Divisão</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -561,6 +606,11 @@
       <c r="C10" t="n">
         <v>10</v>
       </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Primeira Divisão</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -574,6 +624,11 @@
       <c r="C11" t="n">
         <v>16</v>
       </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Primeira Divisão</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -587,6 +642,11 @@
       <c r="C12" t="n">
         <v>11</v>
       </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Primeira Divisão</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -600,6 +660,11 @@
       <c r="C13" t="n">
         <v>4</v>
       </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Primeira Divisão</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -613,6 +678,11 @@
       <c r="C14" t="n">
         <v>14</v>
       </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Primeira Divisão</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -626,6 +696,11 @@
       <c r="C15" t="n">
         <v>1</v>
       </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Primeira Divisão</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -639,6 +714,11 @@
       <c r="C16" t="n">
         <v>5</v>
       </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Primeira Divisão</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -652,6 +732,11 @@
       <c r="C17" t="n">
         <v>4</v>
       </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Primeira Divisão</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -664,6 +749,11 @@
       </c>
       <c r="C18" t="n">
         <v>11</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Primeira Divisão</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>